<commit_message>
Refactor timetable name accurately
</commit_message>
<xml_diff>
--- a/src/main/resources/file/LecturerAvailability.xlsx
+++ b/src/main/resources/file/LecturerAvailability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27930446-C4CC-4A58-AA02-62D01ACF1EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315884B6-9919-4951-9D07-F93DA781EF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,9 +486,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Show detail error messages
</commit_message>
<xml_diff>
--- a/src/main/resources/file/LecturerAvailability.xlsx
+++ b/src/main/resources/file/LecturerAvailability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315884B6-9919-4951-9D07-F93DA781EF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1934B531-B371-4B42-A4AA-C22A405B724E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,7 +472,6 @@
       <c r="C2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="1"/>
       <c r="E2" s="1" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Refactor distance transition fitness to be accurate
</commit_message>
<xml_diff>
--- a/src/main/resources/file/LecturerAvailability.xlsx
+++ b/src/main/resources/file/LecturerAvailability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1934B531-B371-4B42-A4AA-C22A405B724E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D87DE0-07A6-4631-AB46-03951DB1BEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
+    <workbookView xWindow="-21765" yWindow="2760" windowWidth="17280" windowHeight="8880" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,10 +468,6 @@
       <c r="A2" s="1">
         <v>94989873</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="E2" s="1" t="b">
         <v>1</v>
       </c>
@@ -481,11 +477,9 @@
       <c r="A3" s="1">
         <v>78392016</v>
       </c>
-      <c r="B3" s="1" t="b">
+      <c r="D3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
refactor timetablesheetwrite to display all session clearly
</commit_message>
<xml_diff>
--- a/src/main/resources/file/LecturerAvailability.xlsx
+++ b/src/main/resources/file/LecturerAvailability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D87DE0-07A6-4631-AB46-03951DB1BEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F80C907-BB37-4D75-B40C-920D385CFC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21765" yWindow="2760" windowWidth="17280" windowHeight="8880" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,6 +468,7 @@
       <c r="A2" s="1">
         <v>94989873</v>
       </c>
+      <c r="C2" s="1"/>
       <c r="E2" s="1" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Refactor the lecturer and module version
</commit_message>
<xml_diff>
--- a/src/main/resources/file/LecturerAvailability.xlsx
+++ b/src/main/resources/file/LecturerAvailability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F80C907-BB37-4D75-B40C-920D385CFC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6A89C7-CBBF-4B9E-8B69-2C39FBBBDFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
   </bookViews>
@@ -89,10 +89,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C8E56D-40BB-47C0-876A-A176B669BE82}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,6 +471,7 @@
       <c r="A2" s="1">
         <v>94989873</v>
       </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="E2" s="1" t="b">
         <v>1</v>
@@ -478,6 +482,10 @@
       <c r="A3" s="1">
         <v>78392016</v>
       </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="D3" s="1" t="b">
         <v>1</v>
       </c>
@@ -485,6 +493,18 @@
       <c r="F3" s="1" t="b">
         <v>1</v>
       </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>57381920</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactor lecturer and module timetable without redandunt version
</commit_message>
<xml_diff>
--- a/src/main/resources/file/LecturerAvailability.xlsx
+++ b/src/main/resources/file/LecturerAvailability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6A89C7-CBBF-4B9E-8B69-2C39FBBBDFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A82C1EC-73EF-427D-AC02-6252532A246F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
+    <workbookView xWindow="-27840" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,9 +483,7 @@
         <v>78392016</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1" t="b">
         <v>1</v>
       </c>
@@ -495,15 +493,11 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>57381920</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust the weight and improve timetable exporter
</commit_message>
<xml_diff>
--- a/src/main/resources/file/LecturerAvailability.xlsx
+++ b/src/main/resources/file/LecturerAvailability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A82C1EC-73EF-427D-AC02-6252532A246F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9658940-7FD8-4B18-A7E4-0111FDB7B952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27840" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
+    <workbookView xWindow="-25035" yWindow="1815" windowWidth="21600" windowHeight="11235" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,13 +89,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,7 +437,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,33 +474,44 @@
       <c r="A2" s="1">
         <v>94989873</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>78392016</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="b">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4">
+        <v>28374659</v>
+      </c>
+      <c r="B4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="F4" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Perform some test and debug
</commit_message>
<xml_diff>
--- a/src/main/resources/file/LecturerAvailability.xlsx
+++ b/src/main/resources/file/LecturerAvailability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9658940-7FD8-4B18-A7E4-0111FDB7B952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4243591-EC6E-4D19-89E7-47B97AC3AD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25035" yWindow="1815" windowWidth="21600" windowHeight="11235" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
+    <workbookView xWindow="-23190" yWindow="4095" windowWidth="21600" windowHeight="11235" xr2:uid="{81E64A13-B108-466E-BA6A-0A03192CD1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,16 +89,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,7 +434,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,19 +468,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>94989873</v>
       </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="b">
+      <c r="B2" s="2"/>
+      <c r="D2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>78392016</v>
       </c>
       <c r="B3" s="2"/>
@@ -499,16 +499,14 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>28374659</v>
-      </c>
-      <c r="B4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2"/>
+      <c r="A4" s="2">
+        <v>16362061</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="E4" s="2" t="b">
         <v>1</v>
       </c>

</xml_diff>